<commit_message>
set NA value for Nick Saarlos weight
</commit_message>
<xml_diff>
--- a/data/baseballPlayers.xlsx
+++ b/data/baseballPlayers.xlsx
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="baseballPlayers" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/lgreski/gitrepos/datascience/data/baseballPlayers.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/lgreski/gitrepos/datascience/data/baseballPlayers.txt" space="1" consecutive="1">
       <textFields count="6">
         <textField type="text"/>
         <textField type="text"/>
@@ -3599,7 +3599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1019" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A626" workbookViewId="0">
+      <selection activeCell="E643" sqref="E643"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16444,7 +16446,7 @@
       <c r="D642">
         <v>72</v>
       </c>
-      <c r="E642">
+      <c r="F642">
         <v>27.77</v>
       </c>
     </row>

</xml_diff>